<commit_message>
big chunk of work
Last commit in 2023!!!
</commit_message>
<xml_diff>
--- a/MVVMTest/export.xlsx
+++ b/MVVMTest/export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,7 +491,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>7.9 - 7.9</t>
+          <t>1.1 - 2.1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -499,31 +499,11 @@
           <t>1</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>123123</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>123123</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>123123</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>12312</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>12312</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
@@ -534,21 +514,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>18.9 - 18.9</t>
+          <t>28.1 - 31.5</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>123</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>123123</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
@@ -561,19 +537,19 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1.1 - 26.7</t>
+          <t>27.7 - 27.7</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>206</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>asfasf</t>
+          <t>asdfsa23</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -589,7 +565,7 @@
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
-          <t>sdfsdf</t>
+          <t>2df</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -602,92 +578,49 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>27.7 - 27.7</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>asdfsa23</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>234</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>234</t>
-        </is>
-      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>2df</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>234</t>
-        </is>
-      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Сумма:</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Сумма:</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>246246</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>12780</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>12780</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>468</t>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>234</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
animation fixed, need to rebuild launcher
</commit_message>
<xml_diff>
--- a/MVVMTest/export.xlsx
+++ b/MVVMTest/export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,7 +491,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1.1 - 2.1</t>
+          <t>2.1 - 2.1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -514,22 +514,34 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>28.1 - 31.5</t>
+          <t>1.2 - 2.3</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>30</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>9808</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>jkhkjh</t>
+        </is>
+      </c>
       <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -537,7 +549,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>27.7 - 27.7</t>
+          <t>1.1 - 1.1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -549,78 +561,105 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>asdfsa23</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>234</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>234</t>
-        </is>
-      </c>
+          <t>98098080</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>2df</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>234</t>
-        </is>
-      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>27.7 - 27.7</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>asdfsa23</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>2df</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Сумма:</t>
-        </is>
-      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>234</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>234</t>
-        </is>
-      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr">
+      <c r="K6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Сумма:</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>98098080</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>234</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>10042</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>321</t>
         </is>
       </c>
     </row>

</xml_diff>